<commit_message>
Found the conflicting points
It seems that the data point with index 33 was really wrong but the one on 59 is intentional as it is found on the tables. Idk what this meas so lets roll
</commit_message>
<xml_diff>
--- a/eos/data.xlsx
+++ b/eos/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/eos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{2A93DA5E-A402-4EE1-B9F0-18AA1B0E1D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4F8A42FB-B05E-4877-AD12-F50456DE21BE}"/>
+  <xr:revisionPtr revIDLastSave="513" documentId="8_{2A93DA5E-A402-4EE1-B9F0-18AA1B0E1D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC88D48-14EB-45F8-80C5-47176F8A57F8}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17C58B47-18C3-49D3-AB0B-CB9AD996D694}"/>
   </bookViews>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5867ACE-D8BB-4212-8C0B-A23EBDF7BF9E}">
   <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" zoomScale="93" zoomScaleNormal="93" workbookViewId="0">
-      <selection activeCell="D82" sqref="D82"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1669,16 +1669,16 @@
         <v>4.6979999999999999E-3</v>
       </c>
       <c r="B33" s="2">
-        <v>3.5330000000000001E-3</v>
+        <v>3.5329999999999999E-6</v>
       </c>
       <c r="C33" s="2">
-        <v>3.5330000000000001E-3</v>
+        <v>3.5329999999999999E-6</v>
       </c>
       <c r="D33" s="2">
-        <v>3.5330000000000001E-3</v>
+        <v>3.5329999999999999E-6</v>
       </c>
       <c r="E33" s="2">
-        <v>3.5330000000000001E-3</v>
+        <v>3.5329999999999999E-6</v>
       </c>
       <c r="F33" s="2">
         <f t="shared" si="1"/>
@@ -1686,19 +1686,19 @@
       </c>
       <c r="G33" s="2">
         <f t="shared" si="2"/>
-        <v>3.1673521650000003E-9</v>
+        <v>3.1673521650000002E-12</v>
       </c>
       <c r="H33" s="2">
         <f t="shared" si="3"/>
-        <v>3.1673521650000003E-9</v>
+        <v>3.1673521650000002E-12</v>
       </c>
       <c r="I33" s="2">
         <f t="shared" si="4"/>
-        <v>3.1673521650000003E-9</v>
+        <v>3.1673521650000002E-12</v>
       </c>
       <c r="J33" s="2">
         <f t="shared" si="5"/>
-        <v>3.1673521650000003E-9</v>
+        <v>3.1673521650000002E-12</v>
       </c>
       <c r="K33" s="1"/>
     </row>

</xml_diff>

<commit_message>
Changed the logic of the scrypt
Changed it so now instead of calculating and ploting. You needto first calculate and then you plot.
</commit_message>
<xml_diff>
--- a/eos/data.xlsx
+++ b/eos/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/15149eb1c9cf386c/Escritorio/TFG/Codigo-GIT/TFG/eos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="513" documentId="8_{2A93DA5E-A402-4EE1-B9F0-18AA1B0E1D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9BC88D48-14EB-45F8-80C5-47176F8A57F8}"/>
+  <xr:revisionPtr revIDLastSave="514" documentId="8_{2A93DA5E-A402-4EE1-B9F0-18AA1B0E1D1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EA697ACA-15A8-4D02-81C6-02317FC631C7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{17C58B47-18C3-49D3-AB0B-CB9AD996D694}"/>
+    <workbookView xWindow="29760" yWindow="960" windowWidth="21600" windowHeight="11235" xr2:uid="{17C58B47-18C3-49D3-AB0B-CB9AD996D694}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -448,8 +448,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5867ACE-D8BB-4212-8C0B-A23EBDF7BF9E}">
   <dimension ref="A1:K145"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A136" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B145" sqref="B145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,11 +553,11 @@
         <v>5.6506710150000004E-30</v>
       </c>
       <c r="I3" s="2">
-        <f t="shared" ref="I3:I66" si="4">D3*0.000000896505</f>
+        <f>D3*0.000000896505</f>
         <v>5.6506710150000004E-30</v>
       </c>
       <c r="J3" s="2">
-        <f t="shared" ref="J3:J66" si="5">E3*0.000000896505</f>
+        <f t="shared" ref="J3:J66" si="4">E3*0.000000896505</f>
         <v>5.6506710150000004E-30</v>
       </c>
       <c r="K3" s="1"/>
@@ -591,11 +591,11 @@
         <v>5.6506710150000005E-29</v>
       </c>
       <c r="I4" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I3:I66" si="5">D4*0.000000896505</f>
         <v>5.6506710150000005E-29</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.6506710150000005E-29</v>
       </c>
       <c r="K4" s="1"/>
@@ -629,11 +629,11 @@
         <v>6.7695092550000006E-28</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7695092550000006E-28</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.7695092550000006E-28</v>
       </c>
       <c r="K5" s="1"/>
@@ -667,11 +667,11 @@
         <v>7.8327641849999998E-27</v>
       </c>
       <c r="I6" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.8327641849999998E-27</v>
       </c>
       <c r="J6" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.8327641849999998E-27</v>
       </c>
       <c r="K6" s="1"/>
@@ -705,11 +705,11 @@
         <v>9.5119180500000005E-26</v>
       </c>
       <c r="I7" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.5119180500000005E-26</v>
       </c>
       <c r="J7" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.5119180500000005E-26</v>
       </c>
       <c r="K7" s="1"/>
@@ -743,11 +743,11 @@
         <v>3.2561061599999997E-24</v>
       </c>
       <c r="I8" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.2561061599999997E-24</v>
       </c>
       <c r="J8" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.2561061599999997E-24</v>
       </c>
       <c r="K8" s="1"/>
@@ -781,11 +781,11 @@
         <v>1.0632549299999999E-22</v>
       </c>
       <c r="I9" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0632549299999999E-22</v>
       </c>
       <c r="J9" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.0632549299999999E-22</v>
       </c>
       <c r="K9" s="1"/>
@@ -819,11 +819,11 @@
         <v>5.4516469050000003E-21</v>
       </c>
       <c r="I10" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.4516469050000003E-21</v>
       </c>
       <c r="J10" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.4516469050000003E-21</v>
       </c>
       <c r="K10" s="1"/>
@@ -857,11 +857,11 @@
         <v>2.7791655000000003E-20</v>
       </c>
       <c r="I11" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.7791655000000003E-20</v>
       </c>
       <c r="J11" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.7791655000000003E-20</v>
       </c>
       <c r="K11" s="1"/>
@@ -895,11 +895,11 @@
         <v>1.359998085E-19</v>
       </c>
       <c r="I12" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.359998085E-19</v>
       </c>
       <c r="J12" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.359998085E-19</v>
       </c>
       <c r="K12" s="1"/>
@@ -933,11 +933,11 @@
         <v>6.4395954150000001E-19</v>
       </c>
       <c r="I13" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.4395954150000001E-19</v>
       </c>
       <c r="J13" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.4395954150000001E-19</v>
       </c>
       <c r="K13" s="1"/>
@@ -971,11 +971,11 @@
         <v>2.94591543E-18</v>
       </c>
       <c r="I14" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.94591543E-18</v>
       </c>
       <c r="J14" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.94591543E-18</v>
       </c>
       <c r="K14" s="1"/>
@@ -1009,11 +1009,11 @@
         <v>1.297242735E-17</v>
       </c>
       <c r="I15" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.297242735E-17</v>
       </c>
       <c r="J15" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.297242735E-17</v>
       </c>
       <c r="K15" s="1"/>
@@ -1047,11 +1047,11 @@
         <v>5.4579224400000002E-17</v>
       </c>
       <c r="I16" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.4579224400000002E-17</v>
       </c>
       <c r="J16" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.4579224400000002E-17</v>
       </c>
       <c r="K16" s="1"/>
@@ -1085,11 +1085,11 @@
         <v>2.1883687050000003E-16</v>
       </c>
       <c r="I17" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1883687050000003E-16</v>
       </c>
       <c r="J17" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1883687050000003E-16</v>
       </c>
       <c r="K17" s="1"/>
@@ -1123,11 +1123,11 @@
         <v>2.9423294100000003E-16</v>
       </c>
       <c r="I18" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.9423294100000003E-16</v>
       </c>
       <c r="J18" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.9423294100000003E-16</v>
       </c>
       <c r="K18" s="1"/>
@@ -1161,11 +1161,11 @@
         <v>8.0282022749999996E-16</v>
       </c>
       <c r="I19" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.0282022749999996E-16</v>
       </c>
       <c r="J19" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.0282022749999996E-16</v>
       </c>
       <c r="K19" s="1"/>
@@ -1199,11 +1199,11 @@
         <v>2.1444399600000002E-15</v>
       </c>
       <c r="I20" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1444399600000002E-15</v>
       </c>
       <c r="J20" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.1444399600000002E-15</v>
       </c>
       <c r="K20" s="1"/>
@@ -1237,11 +1237,11 @@
         <v>5.62825839E-15</v>
       </c>
       <c r="I21" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.62825839E-15</v>
       </c>
       <c r="J21" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.62825839E-15</v>
       </c>
       <c r="K21" s="1"/>
@@ -1275,11 +1275,11 @@
         <v>1.4568206250000001E-14</v>
       </c>
       <c r="I22" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4568206250000001E-14</v>
       </c>
       <c r="J22" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4568206250000001E-14</v>
       </c>
       <c r="K22" s="1"/>
@@ -1313,11 +1313,11 @@
         <v>3.7348398300000001E-14</v>
       </c>
       <c r="I23" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.7348398300000001E-14</v>
       </c>
       <c r="J23" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.7348398300000001E-14</v>
       </c>
       <c r="K23" s="1"/>
@@ -1351,11 +1351,11 @@
         <v>4.888641765E-14</v>
       </c>
       <c r="I24" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.888641765E-14</v>
       </c>
       <c r="J24" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.888641765E-14</v>
       </c>
       <c r="K24" s="1"/>
@@ -1389,11 +1389,11 @@
         <v>9.1174558500000013E-14</v>
       </c>
       <c r="I25" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9.1174558500000013E-14</v>
       </c>
       <c r="J25" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>9.1174558500000013E-14</v>
       </c>
       <c r="K25" s="1"/>
@@ -1427,11 +1427,11 @@
         <v>1.6943944500000003E-13</v>
       </c>
       <c r="I26" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6943944500000003E-13</v>
       </c>
       <c r="J26" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.6943944500000003E-13</v>
       </c>
       <c r="K26" s="1"/>
@@ -1465,11 +1465,11 @@
         <v>2.3102933850000002E-13</v>
       </c>
       <c r="I27" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.3102933850000002E-13</v>
       </c>
       <c r="J27" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.3102933850000002E-13</v>
       </c>
       <c r="K27" s="1"/>
@@ -1503,11 +1503,11 @@
         <v>2.817715215E-13</v>
       </c>
       <c r="I28" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.817715215E-13</v>
       </c>
       <c r="J28" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.817715215E-13</v>
       </c>
       <c r="K28" s="1"/>
@@ -1541,11 +1541,11 @@
         <v>3.8379379049999999E-13</v>
       </c>
       <c r="I29" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.8379379049999999E-13</v>
       </c>
       <c r="J29" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.8379379049999999E-13</v>
       </c>
       <c r="K29" s="1"/>
@@ -1579,11 +1579,11 @@
         <v>7.1164566900000002E-13</v>
       </c>
       <c r="I30" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.1164566900000002E-13</v>
       </c>
       <c r="J30" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.1164566900000002E-13</v>
       </c>
       <c r="K30" s="1"/>
@@ -1617,11 +1617,11 @@
         <v>1.3178623499999999E-12</v>
       </c>
       <c r="I31" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3178623499999999E-12</v>
       </c>
       <c r="J31" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.3178623499999999E-12</v>
       </c>
       <c r="K31" s="1"/>
@@ -1655,11 +1655,11 @@
         <v>2.44028661E-12</v>
       </c>
       <c r="I32" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.44028661E-12</v>
       </c>
       <c r="J32" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.44028661E-12</v>
       </c>
       <c r="K32" s="1"/>
@@ -1693,11 +1693,11 @@
         <v>3.1673521650000002E-12</v>
       </c>
       <c r="I33" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.1673521650000002E-12</v>
       </c>
       <c r="J33" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.1673521650000002E-12</v>
       </c>
       <c r="K33" s="1"/>
@@ -1731,11 +1731,11 @@
         <v>4.309499535E-12</v>
       </c>
       <c r="I34" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.309499535E-12</v>
       </c>
       <c r="J34" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.309499535E-12</v>
       </c>
       <c r="K34" s="1"/>
@@ -1769,11 +1769,11 @@
         <v>5.8631427000000003E-12</v>
       </c>
       <c r="I35" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.8631427000000003E-12</v>
       </c>
       <c r="J35" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.8631427000000003E-12</v>
       </c>
       <c r="K35" s="1"/>
@@ -1807,11 +1807,11 @@
         <v>7.9726189650000001E-12</v>
       </c>
       <c r="I36" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.9726189650000001E-12</v>
       </c>
       <c r="J36" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.9726189650000001E-12</v>
       </c>
       <c r="K36" s="1"/>
@@ -1845,11 +1845,11 @@
         <v>1.0838745449999999E-11</v>
       </c>
       <c r="I37" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0838745449999999E-11</v>
       </c>
       <c r="J37" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.0838745449999999E-11</v>
       </c>
       <c r="K37" s="1"/>
@@ -1883,11 +1883,11 @@
         <v>1.40034081E-11</v>
       </c>
       <c r="I38" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.40034081E-11</v>
       </c>
       <c r="J38" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.40034081E-11</v>
       </c>
       <c r="K38" s="1"/>
@@ -1921,11 +1921,11 @@
         <v>1.9041766200000001E-11</v>
       </c>
       <c r="I39" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9041766200000001E-11</v>
       </c>
       <c r="J39" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.9041766200000001E-11</v>
       </c>
       <c r="K39" s="1"/>
@@ -1959,11 +1959,11 @@
         <v>2.5891064400000001E-11</v>
       </c>
       <c r="I40" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.5891064400000001E-11</v>
       </c>
       <c r="J40" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.5891064400000001E-11</v>
       </c>
       <c r="K40" s="1"/>
@@ -1997,11 +1997,11 @@
         <v>3.3287230649999998E-11</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.3287230649999998E-11</v>
       </c>
       <c r="J41" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.3287230649999998E-11</v>
       </c>
       <c r="K41" s="1"/>
@@ -2035,11 +2035,11 @@
         <v>4.5255572399999997E-11</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.5255572399999997E-11</v>
       </c>
       <c r="J42" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.5255572399999997E-11</v>
       </c>
       <c r="K42" s="1"/>
@@ -2073,11 +2073,11 @@
         <v>6.1545068250000005E-11</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.1545068250000005E-11</v>
       </c>
       <c r="J43" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.1545068250000005E-11</v>
       </c>
       <c r="K43" s="1"/>
@@ -2111,11 +2111,11 @@
         <v>8.3643916500000004E-11</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8.3643916500000004E-11</v>
       </c>
       <c r="J44" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>8.3643916500000004E-11</v>
       </c>
       <c r="K44" s="1"/>
@@ -2149,11 +2149,11 @@
         <v>1.137664845E-10</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.137664845E-10</v>
       </c>
       <c r="J45" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.137664845E-10</v>
       </c>
       <c r="K45" s="1"/>
@@ -2187,11 +2187,11 @@
         <v>1.4532346050000003E-10</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.4532346050000003E-10</v>
       </c>
       <c r="J46" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.4532346050000003E-10</v>
       </c>
       <c r="K46" s="1"/>
@@ -2225,11 +2225,11 @@
         <v>1.6181915250000001E-10</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6181915250000001E-10</v>
       </c>
       <c r="J47" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.6181915250000001E-10</v>
       </c>
       <c r="K47" s="1"/>
@@ -2263,11 +2263,11 @@
         <v>1.840524765E-10</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.840524765E-10</v>
       </c>
       <c r="J48" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.840524765E-10</v>
       </c>
       <c r="K48" s="1"/>
@@ -2301,11 +2301,11 @@
         <v>2.5021454550000001E-10</v>
       </c>
       <c r="I49" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.5021454550000001E-10</v>
       </c>
       <c r="J49" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.5021454550000001E-10</v>
       </c>
       <c r="K49" s="1"/>
@@ -2339,11 +2339,11 @@
         <v>3.25431315E-10</v>
       </c>
       <c r="I50" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.25431315E-10</v>
       </c>
       <c r="J50" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3.25431315E-10</v>
       </c>
       <c r="K50" s="1"/>
@@ -2377,11 +2377,11 @@
         <v>4.3668758550000004E-10</v>
       </c>
       <c r="I51" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.3668758550000004E-10</v>
       </c>
       <c r="J51" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.3668758550000004E-10</v>
       </c>
       <c r="K51" s="1"/>
@@ -2415,11 +2415,11 @@
         <v>4.4143906200000007E-10</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.4143906200000007E-10</v>
       </c>
       <c r="J52" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.4143906200000007E-10</v>
       </c>
       <c r="K52" s="1"/>
@@ -2453,11 +2453,11 @@
         <v>4.6725840599999997E-10</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.6725840599999997E-10</v>
       </c>
       <c r="J53" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.6725840599999997E-10</v>
       </c>
       <c r="K53" s="1"/>
@@ -2491,11 +2491,11 @@
         <v>5.0903553900000008E-10</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.0903553900000008E-10</v>
       </c>
       <c r="J54" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.0903553900000008E-10</v>
       </c>
       <c r="K54" s="1"/>
@@ -2529,11 +2529,11 @@
         <v>5.5000581750000008E-10</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.5000581750000008E-10</v>
       </c>
       <c r="J55" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.5000581750000008E-10</v>
       </c>
       <c r="K55" s="1"/>
@@ -2567,11 +2567,11 @@
         <v>6.0594772950000001E-10</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.0594772950000001E-10</v>
       </c>
       <c r="J56" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.0594772950000001E-10</v>
       </c>
       <c r="K56" s="1"/>
@@ -2605,11 +2605,11 @@
         <v>6.8143345050000003E-10</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.8143345050000003E-10</v>
       </c>
       <c r="J57" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.8143345050000003E-10</v>
       </c>
       <c r="K57" s="1"/>
@@ -2643,11 +2643,11 @@
         <v>7.8273851550000011E-10</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7.8273851550000011E-10</v>
       </c>
       <c r="J58" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>7.8273851550000011E-10</v>
       </c>
       <c r="K58" s="1"/>
@@ -2681,11 +2681,11 @@
         <v>5.3288257200000009E-10</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3288257200000009E-10</v>
       </c>
       <c r="J59" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.3288257200000009E-10</v>
       </c>
       <c r="K59" s="1"/>
@@ -2719,11 +2719,11 @@
         <v>5.1988324950000004E-9</v>
       </c>
       <c r="I60" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.1988324950000004E-9</v>
       </c>
       <c r="J60" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.1988324950000004E-9</v>
       </c>
       <c r="K60" s="1"/>
@@ -2757,11 +2757,11 @@
         <v>1.0453248300000001E-8</v>
       </c>
       <c r="I61" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.0453248300000001E-8</v>
       </c>
       <c r="J61" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.0453248300000001E-8</v>
       </c>
       <c r="K61" s="1"/>
@@ -2795,11 +2795,11 @@
         <v>1.8692129250000002E-8</v>
       </c>
       <c r="I62" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.8692129250000002E-8</v>
       </c>
       <c r="J62" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1.8692129250000002E-8</v>
       </c>
       <c r="K62" s="1"/>
@@ -2833,11 +2833,11 @@
         <v>2.8831600800000001E-8</v>
       </c>
       <c r="I63" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.8831600800000001E-8</v>
       </c>
       <c r="J63" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2.8831600800000001E-8</v>
       </c>
       <c r="K63" s="1"/>
@@ -2871,11 +2871,11 @@
         <v>4.0477200750000006E-8</v>
       </c>
       <c r="I64" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0477200750000006E-8</v>
       </c>
       <c r="J64" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>4.0477200750000006E-8</v>
       </c>
       <c r="K64" s="1"/>
@@ -2909,11 +2909,11 @@
         <v>5.3440663050000008E-8</v>
       </c>
       <c r="I65" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5.3440663050000008E-8</v>
       </c>
       <c r="J65" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>5.3440663050000008E-8</v>
       </c>
       <c r="K65" s="1"/>
@@ -2947,11 +2947,11 @@
         <v>6.7632337200000001E-8</v>
       </c>
       <c r="I66" s="2">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>6.7632337200000001E-8</v>
       </c>
       <c r="J66" s="2">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>6.7632337200000001E-8</v>
       </c>
       <c r="K66" s="1"/>

</xml_diff>